<commit_message>
Fix for svg/plantuml rendering
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-Appointment.xlsx
+++ b/docs/StructureDefinition-Appointment.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-06T16:19:49+00:00</t>
+    <t>2024-02-07T07:23:51+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1420,17 +1420,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="40.10546875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="40.10546875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.1328125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="5.90234375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.69921875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="39.59375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="39.59375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.3515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="38.4609375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="6.1484375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.58203125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.94140625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="14.7109375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.1875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="91.78515625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="86.96875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1439,27 +1439,27 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="8.84375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="15.71484375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="16.08984375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="17.078125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.3125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="49.39453125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="56.84765625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="17.8203125" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.98828125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="12.3046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="34.0703125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.87890625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="9.04296875" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="15.77734375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="16.13671875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="17.40234375" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.9609375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="48.671875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="57.26953125" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.8828125" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="20.84375" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="18.84765625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="15.703125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="13.125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="33.4296875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.53125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.890625" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="33.4765625" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="106.0703125" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="151.71484375" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="32.84375" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="75.30859375" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="32.98046875" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="104.51171875" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="150.140625" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="33.05078125" customWidth="true" bestFit="true"/>
+    <col min="41" max="41" width="77.2265625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Mock of PMIR IHE UK
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-Appointment.xlsx
+++ b/docs/StructureDefinition-Appointment.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-29T07:38:13+00:00</t>
+    <t>2024-03-05T15:05:36+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1438,17 +1438,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="39.59375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="39.59375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.3515625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="38.4609375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="6.1484375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.58203125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="4.94140625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.7109375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.1875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="40.10546875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="40.10546875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.1328125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.90234375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.69921875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="5.07421875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="86.96875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="91.78515625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1457,27 +1457,27 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="9.04296875" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="15.77734375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="16.13671875" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="17.40234375" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.9609375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="48.671875" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="57.26953125" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.8828125" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="20.84375" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="18.84765625" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="15.703125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="13.125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="33.4296875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.53125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.890625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="8.84375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="15.71484375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="16.08984375" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="17.078125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.3125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="49.39453125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="56.84765625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.69140625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="19.73046875" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="17.8203125" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.98828125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="12.3046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="34.0703125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.87890625" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="32.98046875" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="104.51171875" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="150.140625" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="33.05078125" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="77.2265625" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="33.4765625" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="106.0703125" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="151.71484375" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="32.84375" customWidth="true" bestFit="true"/>
+    <col min="41" max="41" width="75.30859375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
More elab on national proxy and cleaned the admin overview
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-Appointment.xlsx
+++ b/docs/StructureDefinition-Appointment.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-25T16:04:49+00:00</t>
+    <t>2024-03-26T07:33:19+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1438,17 +1438,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="40.10546875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="40.10546875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.1328125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="5.90234375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.69921875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="39.59375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="39.59375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.3515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="38.4609375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="6.1484375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.58203125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.94140625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="14.7109375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.1875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="91.78515625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="86.96875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1457,27 +1457,27 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="8.84375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="15.71484375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="16.08984375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="17.078125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.3125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="49.39453125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="56.84765625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="17.8203125" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.98828125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="12.3046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="34.0703125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.87890625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="9.04296875" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="15.77734375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="16.13671875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="17.40234375" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.9609375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="48.671875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="57.26953125" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.8828125" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="20.84375" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="18.84765625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="15.703125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="13.125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="33.4296875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.53125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.890625" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="33.4765625" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="106.0703125" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="151.71484375" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="32.84375" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="75.30859375" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="32.98046875" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="104.51171875" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="150.140625" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="33.05078125" customWidth="true" bestFit="true"/>
+    <col min="41" max="41" width="77.2265625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Added examples for different parts of the workflow
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-Appointment.xlsx
+++ b/docs/StructureDefinition-Appointment.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-26T07:33:19+00:00</t>
+    <t>2024-03-26T12:37:11+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1438,17 +1438,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="39.59375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="39.59375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.3515625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="38.4609375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="6.1484375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.58203125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="4.94140625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.7109375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.1875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="40.10546875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="40.10546875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.1328125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.90234375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.69921875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="5.07421875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="86.96875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="91.78515625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1457,27 +1457,27 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="9.04296875" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="15.77734375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="16.13671875" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="17.40234375" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.9609375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="48.671875" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="57.26953125" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.8828125" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="20.84375" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="18.84765625" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="15.703125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="13.125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="33.4296875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.53125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.890625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="8.84375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="15.71484375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="16.08984375" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="17.078125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.3125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="49.39453125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="56.84765625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.69140625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="19.73046875" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="17.8203125" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.98828125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="12.3046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="34.0703125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.87890625" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="32.98046875" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="104.51171875" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="150.140625" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="33.05078125" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="77.2265625" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="33.4765625" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="106.0703125" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="151.71484375" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="32.84375" customWidth="true" bestFit="true"/>
+    <col min="41" max="41" width="75.30859375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Updated Patient encounter management pages
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-Appointment.xlsx
+++ b/docs/StructureDefinition-Appointment.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-27T12:02:55+00:00</t>
+    <t>2024-03-28T06:59:04+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1438,17 +1438,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="40.10546875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="40.10546875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.1328125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="5.90234375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.69921875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="39.59375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="39.59375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.3515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="38.4609375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="6.1484375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.58203125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.94140625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="14.7109375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.1875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="91.78515625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="86.96875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1457,27 +1457,27 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="8.84375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="15.71484375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="16.08984375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="17.078125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.3125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="49.39453125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="56.84765625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="17.8203125" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.98828125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="12.3046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="34.0703125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.87890625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="9.04296875" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="15.77734375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="16.13671875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="17.40234375" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.9609375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="48.671875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="57.26953125" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.8828125" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="20.84375" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="18.84765625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="15.703125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="13.125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="33.4296875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.53125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.890625" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="33.4765625" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="106.0703125" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="151.71484375" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="32.84375" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="75.30859375" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="32.98046875" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="104.51171875" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="150.140625" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="33.05078125" customWidth="true" bestFit="true"/>
+    <col min="41" max="41" width="77.2265625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Fag packet of Encounter API
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-Appointment.xlsx
+++ b/docs/StructureDefinition-Appointment.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-04-04T07:58:12+01:00</t>
+    <t>2024-04-09T11:34:38+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1725,17 +1725,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="45.83203125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="45.83203125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.3515625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="38.4609375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="6.1484375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.58203125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="4.94140625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.7109375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.1875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="46.45703125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="46.45703125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.1328125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.90234375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.69921875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="5.07421875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="86.96875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="91.78515625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1744,27 +1744,27 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="38.1875" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="15.77734375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="16.13671875" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="17.40234375" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.9609375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="95.3984375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="57.26953125" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.8828125" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="20.84375" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="40.0859375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="15.703125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="13.125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="33.4296875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.53125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.890625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="38.8125" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="15.71484375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="16.08984375" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="17.078125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.3125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="95.56640625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="56.84765625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.69140625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="19.92578125" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="40.0390625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.98828125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="12.3046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="34.0703125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.87890625" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="32.98046875" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="104.51171875" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="150.140625" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="33.05078125" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="77.2265625" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="33.4765625" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="106.0703125" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="151.71484375" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="32.84375" customWidth="true" bestFit="true"/>
+    <col min="41" max="41" width="75.30859375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>